<commit_message>
Updates R40 : tree view - tabs - datatables
</commit_message>
<xml_diff>
--- a/changelog.xlsx
+++ b/changelog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21105"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Mise à jour</t>
   </si>
@@ -231,6 +231,30 @@
   </si>
   <si>
     <t>/fr/exalead/</t>
+  </si>
+  <si>
+    <t>Ajout du tree view</t>
+  </si>
+  <si>
+    <t>/fr/modules/treeview/</t>
+  </si>
+  <si>
+    <t>Ajout du nouveau système d'onglets</t>
+  </si>
+  <si>
+    <t>/fr/modules/onglets/</t>
+  </si>
+  <si>
+    <t>Mise à jour du module datatables</t>
+  </si>
+  <si>
+    <t>/fr/modules/datatables/</t>
+  </si>
+  <si>
+    <t>Réorganisation de la page index</t>
+  </si>
+  <si>
+    <t>/fr/index.html</t>
   </si>
 </sst>
 </file>
@@ -341,7 +365,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -350,8 +374,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -425,10 +456,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -723,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -765,219 +806,279 @@
         <v>40604</v>
       </c>
       <c r="C3" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="16" customFormat="1">
+      <c r="A4" s="25"/>
+      <c r="B4" s="14">
+        <v>41039</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="16" customFormat="1">
+      <c r="A5" s="25"/>
+      <c r="B5" s="14">
+        <v>41039</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="16" customFormat="1">
+      <c r="A6" s="25"/>
+      <c r="B6" s="14">
+        <v>41039</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="16" customFormat="1">
+      <c r="A7" s="25"/>
+      <c r="B7" s="14">
+        <v>40604</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="15" t="s">
+      <c r="D7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="16" customFormat="1">
-      <c r="A4" s="24"/>
-      <c r="B4" s="14">
+    <row r="8" spans="1:5" s="16" customFormat="1">
+      <c r="A8" s="24"/>
+      <c r="B8" s="14">
         <v>40584</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C8" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="15" t="s">
+      <c r="D8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="16" customFormat="1" ht="28">
-      <c r="A5" s="13" t="s">
+    <row r="9" spans="1:5" s="16" customFormat="1" ht="28">
+      <c r="A9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B9" s="14">
         <v>40226</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E9" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="16" customFormat="1" ht="70">
-      <c r="B6" s="14">
+    <row r="10" spans="1:5" s="16" customFormat="1" ht="70">
+      <c r="B10" s="14">
         <v>40232</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C10" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="18" t="s">
+      <c r="D10" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="19" customFormat="1" ht="70">
-      <c r="B7" s="20">
+    <row r="11" spans="1:5" s="19" customFormat="1" ht="70">
+      <c r="B11" s="20">
         <v>40232</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C11" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="22" t="s">
+      <c r="D11" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="16" customFormat="1" ht="56">
-      <c r="B8" s="14">
+    <row r="12" spans="1:5" s="16" customFormat="1" ht="56">
+      <c r="B12" s="14">
         <v>40239</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C12" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="18" t="s">
+      <c r="D12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="16" customFormat="1" ht="42">
-      <c r="A9" s="13" t="s">
+    <row r="13" spans="1:5" s="16" customFormat="1" ht="42">
+      <c r="A13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B13" s="14">
         <v>40114</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C13" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="15" t="s">
+      <c r="D13" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="9" customFormat="1" ht="36" customHeight="1">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="9" customFormat="1" ht="36" customHeight="1">
-      <c r="B11" s="7"/>
-      <c r="C11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="16" customFormat="1">
-      <c r="A12" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="14">
-        <v>40107</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="9" customFormat="1" ht="23.25" customHeight="1">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="E13" s="8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="9" customFormat="1" ht="36" customHeight="1">
       <c r="B14" s="7"/>
       <c r="C14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="8"/>
+        <v>24</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:5" s="9" customFormat="1" ht="36" customHeight="1">
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" s="9" customFormat="1" ht="36" customHeight="1">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" s="9" customFormat="1" ht="48.75" customHeight="1">
+        <v>26</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="16" customFormat="1">
+      <c r="A16" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="14">
+        <v>40107</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="9" customFormat="1" ht="23.25" customHeight="1">
       <c r="B17" s="7"/>
-      <c r="C17" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="C17" s="8"/>
       <c r="E17" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="9"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="9" customFormat="1" ht="36" customHeight="1">
       <c r="B18" s="7"/>
       <c r="C18" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" s="9" customFormat="1" ht="36" customHeight="1">
+      <c r="B19" s="7"/>
+      <c r="C19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" s="9" customFormat="1" ht="36" customHeight="1">
+      <c r="B20" s="7"/>
+      <c r="C20" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5" s="9" customFormat="1" ht="48.75" customHeight="1">
+      <c r="B21" s="7"/>
+      <c r="C21" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="9"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="8" t="s">
+      <c r="D22" s="9"/>
+      <c r="E22" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="13" t="s">
+    <row r="23" spans="1:5">
+      <c r="A23" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15" t="s">
+      <c r="B23" s="14"/>
+      <c r="C23" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="15" t="s">
+      <c r="D23" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="56">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="12" t="s">
+    <row r="24" spans="1:5" ht="56">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="12" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A3:A8"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E12" r:id="rId1"/>
+    <hyperlink ref="E16" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>